<commit_message>
Update VNpay + createOrder API
</commit_message>
<xml_diff>
--- a/DEPLOY/SOURCE/WEB_API/APIProject/APIProject/Template/List_Customer.xlsx
+++ b/DEPLOY/SOURCE/WEB_API/APIProject/APIProject/Template/List_Customer.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B46879-9060-42F0-AC9C-BFAF02691A12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="3120" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>STT</t>
   </si>
@@ -46,12 +47,15 @@
   </si>
   <si>
     <t>Ví tích điểm</t>
+  </si>
+  <si>
+    <t>Ví V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,11 +441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +456,7 @@
     <col min="9" max="16384" width="25.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -464,7 +468,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -484,17 +488,20 @@
         <v>8</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
     </row>

</xml_diff>